<commit_message>
Firm v0.6 - correcciones y cambios
</commit_message>
<xml_diff>
--- a/Firmware/v0.6 Stable - Hard 0.0/LCD Layout - Firm v06.xlsx
+++ b/Firmware/v0.6 Stable - Hard 0.0/LCD Layout - Firm v06.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="73">
   <si>
     <t>01</t>
   </si>
@@ -629,8 +629,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AF71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="Z49" sqref="Z49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2734,6 +2734,26 @@
       </c>
       <c r="T59" s="1" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R60" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S60" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T60" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U60" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>